<commit_message>
updated typedef to include registering a user. - added task items I believe required to complete project
</commit_message>
<xml_diff>
--- a/documentation/CS554_Final_Project_Planning.xlsx
+++ b/documentation/CS554_Final_Project_Planning.xlsx
@@ -8,19 +8,20 @@
       <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="C:\Users\vazqu\Documents\Stevens\Assignments\CS554-Final-Project\documentation\"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{172656AF-9F45-4BCD-9D5A-E2C96FB70856}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
+  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{C1732A5E-4716-48E7-A04B-F20A435CE00F}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
-    <workbookView xWindow="-23610" yWindow="-1110" windowWidth="23610" windowHeight="14325" firstSheet="3" activeTab="6" xr2:uid="{BACD6A66-4D44-40DF-9AFF-EF3917B1C16B}"/>
+    <workbookView xWindow="-30495" yWindow="-8325" windowWidth="26205" windowHeight="18495" tabRatio="937" xr2:uid="{BACD6A66-4D44-40DF-9AFF-EF3917B1C16B}"/>
   </bookViews>
   <sheets>
-    <sheet name="App Component" sheetId="5" r:id="rId1"/>
-    <sheet name="Navigation Bar Component" sheetId="3" r:id="rId2"/>
-    <sheet name="Login Modal" sheetId="6" r:id="rId3"/>
-    <sheet name="Image Sharing Component" sheetId="4" r:id="rId4"/>
-    <sheet name="Share Image Modal" sheetId="11" r:id="rId5"/>
-    <sheet name="Posted Image Component" sheetId="8" r:id="rId6"/>
-    <sheet name="Image Creation Component" sheetId="9" r:id="rId7"/>
-    <sheet name="Create Image Modal" sheetId="10" r:id="rId8"/>
+    <sheet name="Todo" sheetId="12" r:id="rId1"/>
+    <sheet name="App Component" sheetId="5" r:id="rId2"/>
+    <sheet name="Navigation Bar Component" sheetId="3" r:id="rId3"/>
+    <sheet name="Login Modal" sheetId="6" r:id="rId4"/>
+    <sheet name="Image Sharing Component" sheetId="4" r:id="rId5"/>
+    <sheet name="Share Image Modal" sheetId="11" r:id="rId6"/>
+    <sheet name="Posted Image Component" sheetId="8" r:id="rId7"/>
+    <sheet name="Image Creation Component" sheetId="9" r:id="rId8"/>
+    <sheet name="Create Image Modal" sheetId="10" r:id="rId9"/>
   </sheets>
   <calcPr calcId="191029"/>
   <extLst>
@@ -43,7 +44,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="100" uniqueCount="64">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="117" uniqueCount="80">
   <si>
     <t>React Item</t>
   </si>
@@ -235,6 +236,54 @@
   </si>
   <si>
     <t>Created Image List</t>
+  </si>
+  <si>
+    <t>Task #</t>
+  </si>
+  <si>
+    <t>Owner</t>
+  </si>
+  <si>
+    <t>Status</t>
+  </si>
+  <si>
+    <t>Define typeDef to establish database</t>
+  </si>
+  <si>
+    <t>Build app component</t>
+  </si>
+  <si>
+    <t>Build navigation component</t>
+  </si>
+  <si>
+    <t>build login modal</t>
+  </si>
+  <si>
+    <t>build image sharing component</t>
+  </si>
+  <si>
+    <t>build image creation component</t>
+  </si>
+  <si>
+    <t>build leaderboard component</t>
+  </si>
+  <si>
+    <t>build logout modal</t>
+  </si>
+  <si>
+    <t>create addSharedImage mutation</t>
+  </si>
+  <si>
+    <t>create removeSharedImage mutation</t>
+  </si>
+  <si>
+    <t>create addCreatedImage mutation</t>
+  </si>
+  <si>
+    <t>create removeCreatedImage mutation</t>
+  </si>
+  <si>
+    <t>create registerUser mutation</t>
   </si>
 </sst>
 </file>
@@ -605,11 +654,232 @@
 </file>
 
 <file path=xl/worksheets/sheet1.xml><?xml version="1.0" encoding="utf-8"?>
+<worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{D1CE48B0-4129-402B-B324-23A2E135981A}">
+  <dimension ref="A1:D31"/>
+  <sheetViews>
+    <sheetView tabSelected="1" workbookViewId="0">
+      <selection activeCell="B5" sqref="B4:B5"/>
+    </sheetView>
+  </sheetViews>
+  <sheetFormatPr defaultRowHeight="15" x14ac:dyDescent="0.25"/>
+  <cols>
+    <col min="2" max="2" width="116.140625" customWidth="1"/>
+  </cols>
+  <sheetData>
+    <row r="1" spans="1:4" x14ac:dyDescent="0.25">
+      <c r="A1" t="s">
+        <v>64</v>
+      </c>
+      <c r="B1" t="s">
+        <v>6</v>
+      </c>
+      <c r="C1" t="s">
+        <v>65</v>
+      </c>
+      <c r="D1" t="s">
+        <v>66</v>
+      </c>
+    </row>
+    <row r="2" spans="1:4" x14ac:dyDescent="0.25">
+      <c r="A2">
+        <v>1</v>
+      </c>
+      <c r="B2" t="s">
+        <v>67</v>
+      </c>
+    </row>
+    <row r="3" spans="1:4" x14ac:dyDescent="0.25">
+      <c r="A3">
+        <v>2</v>
+      </c>
+      <c r="B3" t="s">
+        <v>68</v>
+      </c>
+    </row>
+    <row r="4" spans="1:4" x14ac:dyDescent="0.25">
+      <c r="A4">
+        <v>3</v>
+      </c>
+      <c r="B4" t="s">
+        <v>69</v>
+      </c>
+    </row>
+    <row r="5" spans="1:4" x14ac:dyDescent="0.25">
+      <c r="A5">
+        <v>4</v>
+      </c>
+      <c r="B5" t="s">
+        <v>70</v>
+      </c>
+    </row>
+    <row r="6" spans="1:4" x14ac:dyDescent="0.25">
+      <c r="A6">
+        <v>5</v>
+      </c>
+      <c r="B6" t="s">
+        <v>74</v>
+      </c>
+    </row>
+    <row r="7" spans="1:4" x14ac:dyDescent="0.25">
+      <c r="A7">
+        <v>6</v>
+      </c>
+      <c r="B7" t="s">
+        <v>71</v>
+      </c>
+    </row>
+    <row r="8" spans="1:4" x14ac:dyDescent="0.25">
+      <c r="A8">
+        <v>7</v>
+      </c>
+      <c r="B8" t="s">
+        <v>72</v>
+      </c>
+    </row>
+    <row r="9" spans="1:4" x14ac:dyDescent="0.25">
+      <c r="A9">
+        <v>8</v>
+      </c>
+      <c r="B9" t="s">
+        <v>73</v>
+      </c>
+    </row>
+    <row r="10" spans="1:4" x14ac:dyDescent="0.25">
+      <c r="A10">
+        <v>9</v>
+      </c>
+      <c r="B10" t="s">
+        <v>75</v>
+      </c>
+    </row>
+    <row r="11" spans="1:4" x14ac:dyDescent="0.25">
+      <c r="A11">
+        <v>10</v>
+      </c>
+      <c r="B11" t="s">
+        <v>76</v>
+      </c>
+    </row>
+    <row r="12" spans="1:4" x14ac:dyDescent="0.25">
+      <c r="A12">
+        <v>11</v>
+      </c>
+      <c r="B12" t="s">
+        <v>77</v>
+      </c>
+    </row>
+    <row r="13" spans="1:4" x14ac:dyDescent="0.25">
+      <c r="A13">
+        <v>12</v>
+      </c>
+      <c r="B13" t="s">
+        <v>78</v>
+      </c>
+    </row>
+    <row r="14" spans="1:4" x14ac:dyDescent="0.25">
+      <c r="A14">
+        <v>13</v>
+      </c>
+      <c r="B14" t="s">
+        <v>79</v>
+      </c>
+    </row>
+    <row r="15" spans="1:4" x14ac:dyDescent="0.25">
+      <c r="A15">
+        <v>14</v>
+      </c>
+    </row>
+    <row r="16" spans="1:4" x14ac:dyDescent="0.25">
+      <c r="A16">
+        <v>15</v>
+      </c>
+    </row>
+    <row r="17" spans="1:1" x14ac:dyDescent="0.25">
+      <c r="A17">
+        <v>16</v>
+      </c>
+    </row>
+    <row r="18" spans="1:1" x14ac:dyDescent="0.25">
+      <c r="A18">
+        <v>17</v>
+      </c>
+    </row>
+    <row r="19" spans="1:1" x14ac:dyDescent="0.25">
+      <c r="A19">
+        <v>18</v>
+      </c>
+    </row>
+    <row r="20" spans="1:1" x14ac:dyDescent="0.25">
+      <c r="A20">
+        <v>19</v>
+      </c>
+    </row>
+    <row r="21" spans="1:1" x14ac:dyDescent="0.25">
+      <c r="A21">
+        <v>20</v>
+      </c>
+    </row>
+    <row r="22" spans="1:1" x14ac:dyDescent="0.25">
+      <c r="A22">
+        <v>21</v>
+      </c>
+    </row>
+    <row r="23" spans="1:1" x14ac:dyDescent="0.25">
+      <c r="A23">
+        <v>22</v>
+      </c>
+    </row>
+    <row r="24" spans="1:1" x14ac:dyDescent="0.25">
+      <c r="A24">
+        <v>23</v>
+      </c>
+    </row>
+    <row r="25" spans="1:1" x14ac:dyDescent="0.25">
+      <c r="A25">
+        <v>24</v>
+      </c>
+    </row>
+    <row r="26" spans="1:1" x14ac:dyDescent="0.25">
+      <c r="A26">
+        <v>25</v>
+      </c>
+    </row>
+    <row r="27" spans="1:1" x14ac:dyDescent="0.25">
+      <c r="A27">
+        <v>26</v>
+      </c>
+    </row>
+    <row r="28" spans="1:1" x14ac:dyDescent="0.25">
+      <c r="A28">
+        <v>27</v>
+      </c>
+    </row>
+    <row r="29" spans="1:1" x14ac:dyDescent="0.25">
+      <c r="A29">
+        <v>28</v>
+      </c>
+    </row>
+    <row r="30" spans="1:1" x14ac:dyDescent="0.25">
+      <c r="A30">
+        <v>29</v>
+      </c>
+    </row>
+    <row r="31" spans="1:1" x14ac:dyDescent="0.25">
+      <c r="A31">
+        <v>30</v>
+      </c>
+    </row>
+  </sheetData>
+  <pageMargins left="0.7" right="0.7" top="0.75" bottom="0.75" header="0.3" footer="0.3"/>
+</worksheet>
+</file>
+
+<file path=xl/worksheets/sheet2.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{2A428F30-A303-4DD1-B094-F15F38B78A7A}">
   <dimension ref="A1:C3"/>
   <sheetViews>
     <sheetView workbookViewId="0">
-      <selection activeCell="D19" sqref="D19"/>
+      <selection activeCell="F37" sqref="F37"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="15" x14ac:dyDescent="0.25"/>
@@ -656,7 +926,7 @@
 </worksheet>
 </file>
 
-<file path=xl/worksheets/sheet2.xml><?xml version="1.0" encoding="utf-8"?>
+<file path=xl/worksheets/sheet3.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{F9662216-429F-4ADB-86BD-88D30D231471}">
   <dimension ref="A1:C6"/>
   <sheetViews>
@@ -742,12 +1012,12 @@
 </worksheet>
 </file>
 
-<file path=xl/worksheets/sheet3.xml><?xml version="1.0" encoding="utf-8"?>
+<file path=xl/worksheets/sheet4.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{882852A1-A1E8-4C93-AEFC-50026EB54DB8}">
   <dimension ref="A1:C5"/>
   <sheetViews>
     <sheetView workbookViewId="0">
-      <selection activeCell="B9" sqref="B9"/>
+      <selection activeCell="D44" sqref="D44"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="15" x14ac:dyDescent="0.25"/>
@@ -811,7 +1081,7 @@
 </worksheet>
 </file>
 
-<file path=xl/worksheets/sheet4.xml><?xml version="1.0" encoding="utf-8"?>
+<file path=xl/worksheets/sheet5.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{DD7765ED-DE4C-4385-B337-895CEDE71D01}">
   <dimension ref="A1:C3"/>
   <sheetViews>
@@ -864,7 +1134,7 @@
 </worksheet>
 </file>
 
-<file path=xl/worksheets/sheet5.xml><?xml version="1.0" encoding="utf-8"?>
+<file path=xl/worksheets/sheet6.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{AF0B2435-353F-4AA3-B47B-A728B2B3366E}">
   <dimension ref="A1:C4"/>
   <sheetViews>
@@ -927,7 +1197,7 @@
 </worksheet>
 </file>
 
-<file path=xl/worksheets/sheet6.xml><?xml version="1.0" encoding="utf-8"?>
+<file path=xl/worksheets/sheet7.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{2E164DC8-7831-4B34-8019-C78ECEDD268E}">
   <dimension ref="A1:C4"/>
   <sheetViews>
@@ -991,11 +1261,11 @@
 </worksheet>
 </file>
 
-<file path=xl/worksheets/sheet7.xml><?xml version="1.0" encoding="utf-8"?>
+<file path=xl/worksheets/sheet8.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{B6705706-C517-4DB0-9640-3A85F9F452EC}">
   <dimension ref="A1:C3"/>
   <sheetViews>
-    <sheetView tabSelected="1" workbookViewId="0">
+    <sheetView workbookViewId="0">
       <selection activeCell="C16" sqref="C16"/>
     </sheetView>
   </sheetViews>
@@ -1044,7 +1314,7 @@
 </worksheet>
 </file>
 
-<file path=xl/worksheets/sheet8.xml><?xml version="1.0" encoding="utf-8"?>
+<file path=xl/worksheets/sheet9.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{BEB55AB5-63BD-4223-AC3F-6E13556CE159}">
   <dimension ref="A1:C6"/>
   <sheetViews>

</xml_diff>

<commit_message>
updated documentation and .gitignore
</commit_message>
<xml_diff>
--- a/documentation/CS554_Final_Project_Planning.xlsx
+++ b/documentation/CS554_Final_Project_Planning.xlsx
@@ -8,9 +8,9 @@
       <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="C:\Users\vazqu\Documents\Stevens\Assignments\CS554-Final-Project\documentation\"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{C1732A5E-4716-48E7-A04B-F20A435CE00F}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
+  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{E9AFA7D3-8A50-4E2A-9D2E-E0ED7CBA0700}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
-    <workbookView xWindow="-30495" yWindow="-8325" windowWidth="26205" windowHeight="18495" tabRatio="937" xr2:uid="{BACD6A66-4D44-40DF-9AFF-EF3917B1C16B}"/>
+    <workbookView xWindow="-28620" yWindow="-7680" windowWidth="27930" windowHeight="18495" tabRatio="937" xr2:uid="{BACD6A66-4D44-40DF-9AFF-EF3917B1C16B}"/>
   </bookViews>
   <sheets>
     <sheet name="Todo" sheetId="12" r:id="rId1"/>
@@ -44,7 +44,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="117" uniqueCount="80">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="130" uniqueCount="86">
   <si>
     <t>React Item</t>
   </si>
@@ -284,6 +284,24 @@
   </si>
   <si>
     <t>create registerUser mutation</t>
+  </si>
+  <si>
+    <t>Completeish</t>
+  </si>
+  <si>
+    <t>Jameson Riley</t>
+  </si>
+  <si>
+    <t>Naseem</t>
+  </si>
+  <si>
+    <t>Steven</t>
+  </si>
+  <si>
+    <t>Andrew</t>
+  </si>
+  <si>
+    <t>Naseem/Andrew</t>
   </si>
 </sst>
 </file>
@@ -657,13 +675,15 @@
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{D1CE48B0-4129-402B-B324-23A2E135981A}">
   <dimension ref="A1:D31"/>
   <sheetViews>
-    <sheetView tabSelected="1" workbookViewId="0">
-      <selection activeCell="B5" sqref="B4:B5"/>
+    <sheetView tabSelected="1" zoomScale="190" zoomScaleNormal="190" workbookViewId="0">
+      <selection activeCell="B11" sqref="B11"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="15" x14ac:dyDescent="0.25"/>
   <cols>
-    <col min="2" max="2" width="116.140625" customWidth="1"/>
+    <col min="2" max="2" width="78" customWidth="1"/>
+    <col min="3" max="3" width="13.5703125" bestFit="1" customWidth="1"/>
+    <col min="4" max="4" width="12" bestFit="1" customWidth="1"/>
   </cols>
   <sheetData>
     <row r="1" spans="1:4" x14ac:dyDescent="0.25">
@@ -687,6 +707,9 @@
       <c r="B2" t="s">
         <v>67</v>
       </c>
+      <c r="D2" t="s">
+        <v>80</v>
+      </c>
     </row>
     <row r="3" spans="1:4" x14ac:dyDescent="0.25">
       <c r="A3">
@@ -695,6 +718,9 @@
       <c r="B3" t="s">
         <v>68</v>
       </c>
+      <c r="D3" t="s">
+        <v>80</v>
+      </c>
     </row>
     <row r="4" spans="1:4" x14ac:dyDescent="0.25">
       <c r="A4">
@@ -703,6 +729,9 @@
       <c r="B4" t="s">
         <v>69</v>
       </c>
+      <c r="D4" t="s">
+        <v>80</v>
+      </c>
     </row>
     <row r="5" spans="1:4" x14ac:dyDescent="0.25">
       <c r="A5">
@@ -711,6 +740,9 @@
       <c r="B5" t="s">
         <v>70</v>
       </c>
+      <c r="C5" t="s">
+        <v>81</v>
+      </c>
     </row>
     <row r="6" spans="1:4" x14ac:dyDescent="0.25">
       <c r="A6">
@@ -719,6 +751,9 @@
       <c r="B6" t="s">
         <v>74</v>
       </c>
+      <c r="C6" t="s">
+        <v>81</v>
+      </c>
     </row>
     <row r="7" spans="1:4" x14ac:dyDescent="0.25">
       <c r="A7">
@@ -727,6 +762,9 @@
       <c r="B7" t="s">
         <v>71</v>
       </c>
+      <c r="C7" t="s">
+        <v>84</v>
+      </c>
     </row>
     <row r="8" spans="1:4" x14ac:dyDescent="0.25">
       <c r="A8">
@@ -735,6 +773,9 @@
       <c r="B8" t="s">
         <v>72</v>
       </c>
+      <c r="C8" t="s">
+        <v>85</v>
+      </c>
     </row>
     <row r="9" spans="1:4" x14ac:dyDescent="0.25">
       <c r="A9">
@@ -743,6 +784,9 @@
       <c r="B9" t="s">
         <v>73</v>
       </c>
+      <c r="C9" t="s">
+        <v>82</v>
+      </c>
     </row>
     <row r="10" spans="1:4" x14ac:dyDescent="0.25">
       <c r="A10">
@@ -751,6 +795,9 @@
       <c r="B10" t="s">
         <v>75</v>
       </c>
+      <c r="C10" t="s">
+        <v>83</v>
+      </c>
     </row>
     <row r="11" spans="1:4" x14ac:dyDescent="0.25">
       <c r="A11">
@@ -759,6 +806,9 @@
       <c r="B11" t="s">
         <v>76</v>
       </c>
+      <c r="C11" t="s">
+        <v>83</v>
+      </c>
     </row>
     <row r="12" spans="1:4" x14ac:dyDescent="0.25">
       <c r="A12">
@@ -767,6 +817,9 @@
       <c r="B12" t="s">
         <v>77</v>
       </c>
+      <c r="C12" t="s">
+        <v>83</v>
+      </c>
     </row>
     <row r="13" spans="1:4" x14ac:dyDescent="0.25">
       <c r="A13">
@@ -775,6 +828,9 @@
       <c r="B13" t="s">
         <v>78</v>
       </c>
+      <c r="C13" t="s">
+        <v>83</v>
+      </c>
     </row>
     <row r="14" spans="1:4" x14ac:dyDescent="0.25">
       <c r="A14">
@@ -782,6 +838,9 @@
       </c>
       <c r="B14" t="s">
         <v>79</v>
+      </c>
+      <c r="C14" t="s">
+        <v>81</v>
       </c>
     </row>
     <row r="15" spans="1:4" x14ac:dyDescent="0.25">

</xml_diff>